<commit_message>
feat: added readme and fine tuned logs
</commit_message>
<xml_diff>
--- a/Data/Input/CompanyList.xlsx
+++ b/Data/Input/CompanyList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\StockPrice\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\CompanyStockInfo\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Aditya Birla F</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>DFL</t>
+  </si>
+  <si>
+    <t>ABC</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -412,22 +415,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -437,32 +445,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:A5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>